<commit_message>
375 Layer Generator Rev2
</commit_message>
<xml_diff>
--- a/375_FOB_BL_layergenerator.xlsx
+++ b/375_FOB_BL_layergenerator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claudi.marti\Documents\GitHub\Getsend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claudi.marti\Documents\GitHub\Getsend\GetSend_380\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2324" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="652">
   <si>
     <t>TAGNAME</t>
   </si>
@@ -1985,12 +1985,6 @@
   </si>
   <si>
     <t>R7040_1A_Overview_Display.xaml</t>
-  </si>
-  <si>
-    <t>Temp_MRU7990</t>
-  </si>
-  <si>
-    <t>XA799013</t>
   </si>
   <si>
     <t>7990B</t>
@@ -6595,10 +6589,10 @@
   <dimension ref="A1:J226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C173" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B224" sqref="B224"/>
+      <selection pane="bottomRight" activeCell="D226" sqref="D226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -11934,14 +11928,8 @@
       </c>
     </row>
     <row r="224" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B224" s="4" t="s">
-        <v>651</v>
-      </c>
       <c r="C224" t="s">
         <v>172</v>
-      </c>
-      <c r="D224" t="s">
-        <v>647</v>
       </c>
       <c r="E224" t="s">
         <v>7</v>
@@ -11961,9 +11949,6 @@
       </c>
     </row>
     <row r="226" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B226" s="4" t="s">
-        <v>652</v>
-      </c>
       <c r="C226" t="s">
         <v>267</v>
       </c>
@@ -11971,7 +11956,7 @@
         <v>7</v>
       </c>
       <c r="F226" s="6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="H226">
         <v>3</v>

</xml_diff>